<commit_message>
Update 324684580 Apple Store Reviews.xlsx
</commit_message>
<xml_diff>
--- a/324684580 Apple Store Reviews.xlsx
+++ b/324684580 Apple Store Reviews.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2399a590dab840c7/Desktop/Repositories/apple-store-data-collector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_5E4997875B80D42E13F82E11595ED87656C097C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE23C653-8D96-4C3E-91F5-43B6716BE9AB}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_5E4997875B80D42E13F82E11595ED87656C097C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F769128F-4ADF-47D2-A451-2A5CE7E6BFD0}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2928" yWindow="2928" windowWidth="15552" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$501</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -10315,9 +10318,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D377" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G501"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -10362,7 +10368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -10403,7 +10409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10444,7 +10450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -10485,7 +10491,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -10526,7 +10532,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -10567,7 +10573,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -10608,7 +10614,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -10649,7 +10655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -10690,7 +10696,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -10772,7 +10778,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -10813,7 +10819,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -10854,7 +10860,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -10895,7 +10901,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -10936,7 +10942,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -11018,7 +11024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -11059,7 +11065,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -11100,7 +11106,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -11141,7 +11147,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -11182,7 +11188,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -11223,7 +11229,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -11264,7 +11270,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -11305,7 +11311,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -11428,7 +11434,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -11510,7 +11516,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -11551,7 +11557,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -11592,7 +11598,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -11633,7 +11639,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -11674,7 +11680,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -11715,7 +11721,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -11838,7 +11844,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -11879,7 +11885,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -11920,7 +11926,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -12002,7 +12008,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -12084,7 +12090,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -12125,7 +12131,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -12166,7 +12172,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -12207,7 +12213,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -12248,7 +12254,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -12289,7 +12295,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -12330,7 +12336,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -12412,7 +12418,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -12453,7 +12459,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -12494,7 +12500,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -12535,7 +12541,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -12576,7 +12582,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -12658,7 +12664,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -12740,7 +12746,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -12781,7 +12787,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -12822,7 +12828,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -12863,7 +12869,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -12904,7 +12910,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -12986,7 +12992,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -13068,7 +13074,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -13109,7 +13115,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -13191,7 +13197,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -13232,7 +13238,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -13273,7 +13279,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -13396,7 +13402,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -13437,7 +13443,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -13478,7 +13484,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -13519,7 +13525,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -13560,7 +13566,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -13601,7 +13607,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -13642,7 +13648,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -13683,7 +13689,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -13724,7 +13730,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -13765,7 +13771,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -14011,7 +14017,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -14052,7 +14058,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -14093,7 +14099,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -14134,7 +14140,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -14175,7 +14181,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -14216,7 +14222,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -14257,7 +14263,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -14339,7 +14345,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -14421,7 +14427,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -14462,7 +14468,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -14503,7 +14509,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -14544,7 +14550,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -14585,7 +14591,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -14626,7 +14632,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -14667,7 +14673,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -14708,7 +14714,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -14749,7 +14755,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -14790,7 +14796,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -14831,7 +14837,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -14872,7 +14878,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -14954,7 +14960,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -14995,7 +15001,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -15118,7 +15124,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -15159,7 +15165,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -15200,7 +15206,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -15241,7 +15247,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -15282,7 +15288,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -15323,7 +15329,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -15364,7 +15370,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -15446,7 +15452,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -15487,7 +15493,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -15528,7 +15534,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -15569,7 +15575,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -15610,7 +15616,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -15651,7 +15657,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -15733,7 +15739,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -15815,7 +15821,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -15856,7 +15862,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -15897,7 +15903,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -15938,7 +15944,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -15979,7 +15985,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -16020,7 +16026,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -16061,7 +16067,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -16102,7 +16108,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -16143,7 +16149,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -16184,7 +16190,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -16225,7 +16231,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -16266,7 +16272,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -16307,7 +16313,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -16389,7 +16395,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -16430,7 +16436,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -16512,7 +16518,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -16553,7 +16559,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -16594,7 +16600,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -16635,7 +16641,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -16676,7 +16682,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -16717,7 +16723,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -16758,7 +16764,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -16799,7 +16805,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -16840,7 +16846,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -16881,7 +16887,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -16922,7 +16928,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -16963,7 +16969,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -17004,7 +17010,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -17045,7 +17051,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -17086,7 +17092,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -17127,7 +17133,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -17168,7 +17174,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -17209,7 +17215,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -17250,7 +17256,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -17291,7 +17297,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -17332,7 +17338,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -17373,7 +17379,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -17414,7 +17420,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -17496,7 +17502,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -17537,7 +17543,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -17660,7 +17666,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -17783,7 +17789,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -17824,7 +17830,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -17865,7 +17871,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -17947,7 +17953,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -17988,7 +17994,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -18029,7 +18035,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -18070,7 +18076,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -18111,7 +18117,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -18152,7 +18158,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -18193,7 +18199,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -18234,7 +18240,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -18275,7 +18281,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -18316,7 +18322,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -18357,7 +18363,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -18398,7 +18404,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -18439,7 +18445,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -18480,7 +18486,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -18521,7 +18527,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -18562,7 +18568,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -18603,7 +18609,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -18644,7 +18650,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -18685,7 +18691,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -18726,7 +18732,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -18767,7 +18773,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -18808,7 +18814,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -18849,7 +18855,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -18931,7 +18937,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -18972,7 +18978,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -19054,7 +19060,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -19259,7 +19265,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -19300,7 +19306,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -19382,7 +19388,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -19423,7 +19429,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -19505,7 +19511,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -19587,7 +19593,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -19628,7 +19634,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -19669,7 +19675,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -19751,7 +19757,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -19792,7 +19798,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -19833,7 +19839,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -19874,7 +19880,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -19997,7 +20003,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -20038,7 +20044,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -20120,7 +20126,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -20161,7 +20167,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -20243,7 +20249,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -20284,7 +20290,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -20325,7 +20331,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -20366,7 +20372,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -20407,7 +20413,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -20530,7 +20536,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -20612,7 +20618,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -20653,7 +20659,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -20735,7 +20741,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -20817,7 +20823,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -20858,7 +20864,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -20899,7 +20905,7 @@
         <v>1726</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -20981,7 +20987,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -21063,7 +21069,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -21104,7 +21110,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -21186,7 +21192,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -21268,7 +21274,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -21350,7 +21356,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -21391,7 +21397,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -21473,7 +21479,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -21514,7 +21520,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -21637,7 +21643,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -21678,7 +21684,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -21719,7 +21725,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -21801,7 +21807,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -21842,7 +21848,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -21924,7 +21930,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -22047,7 +22053,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -22088,7 +22094,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -22129,7 +22135,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -22211,7 +22217,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -22252,7 +22258,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -22334,7 +22340,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -22375,7 +22381,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -22457,7 +22463,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -22498,7 +22504,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -22539,7 +22545,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -22580,7 +22586,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -22662,7 +22668,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -22703,7 +22709,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -22744,7 +22750,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -22785,7 +22791,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -22826,7 +22832,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -22867,7 +22873,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -22908,7 +22914,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -22990,7 +22996,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -23031,7 +23037,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -23072,7 +23078,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -23113,7 +23119,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -23154,7 +23160,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -23195,7 +23201,7 @@
         <v>2074</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -23277,7 +23283,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -23318,7 +23324,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -23359,7 +23365,7 @@
         <v>2097</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -23400,7 +23406,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -23523,7 +23529,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -23564,7 +23570,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -23605,7 +23611,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -23646,7 +23652,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -23728,7 +23734,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -23769,7 +23775,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -23810,7 +23816,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -23851,7 +23857,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -23892,7 +23898,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -23933,7 +23939,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -23974,7 +23980,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -24056,7 +24062,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -24097,7 +24103,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -24138,7 +24144,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -24220,7 +24226,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -24261,7 +24267,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -24302,7 +24308,7 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -24343,7 +24349,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -24384,7 +24390,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -24425,7 +24431,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -24466,7 +24472,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -24548,7 +24554,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -24589,7 +24595,7 @@
         <v>2276</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -24630,7 +24636,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -24712,7 +24718,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -24753,7 +24759,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -24794,7 +24800,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -24835,7 +24841,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -24876,7 +24882,7 @@
         <v>2317</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -24917,7 +24923,7 @@
         <v>2323</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -24958,7 +24964,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -24999,7 +25005,7 @@
         <v>2336</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -25040,7 +25046,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -25081,7 +25087,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -25122,7 +25128,7 @@
         <v>2356</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -25163,7 +25169,7 @@
         <v>2363</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -25204,7 +25210,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -25286,7 +25292,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -25327,7 +25333,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -25409,7 +25415,7 @@
         <v>2398</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -25450,7 +25456,7 @@
         <v>2404</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -25532,7 +25538,7 @@
         <v>2415</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -25573,7 +25579,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -25614,7 +25620,7 @@
         <v>2427</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -25655,7 +25661,7 @@
         <v>2433</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -25696,7 +25702,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -25819,7 +25825,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -25860,7 +25866,7 @@
         <v>2463</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -25901,7 +25907,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -25983,7 +25989,7 @@
         <v>2481</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -26024,7 +26030,7 @@
         <v>2487</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -26065,7 +26071,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -26147,7 +26153,7 @@
         <v>2505</v>
       </c>
     </row>
-    <row r="387" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -26188,7 +26194,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -26270,7 +26276,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="390" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -26311,7 +26317,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -26352,7 +26358,7 @@
         <v>2535</v>
       </c>
     </row>
-    <row r="392" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -26393,7 +26399,7 @@
         <v>2541</v>
       </c>
     </row>
-    <row r="393" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -26475,7 +26481,7 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -26516,7 +26522,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -26557,7 +26563,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="397" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -26598,7 +26604,7 @@
         <v>2573</v>
       </c>
     </row>
-    <row r="398" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -26639,7 +26645,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -26680,7 +26686,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -26721,7 +26727,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -26762,7 +26768,7 @@
         <v>2596</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -26926,7 +26932,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -26967,7 +26973,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -27008,7 +27014,7 @@
         <v>2632</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -27049,7 +27055,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -27090,7 +27096,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -27131,7 +27137,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -27172,7 +27178,7 @@
         <v>2658</v>
       </c>
     </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -27213,7 +27219,7 @@
         <v>2664</v>
       </c>
     </row>
-    <row r="413" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -27254,7 +27260,7 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -27295,7 +27301,7 @@
         <v>2677</v>
       </c>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -27377,7 +27383,7 @@
         <v>2688</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -27418,7 +27424,7 @@
         <v>2694</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -27500,7 +27506,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -27541,7 +27547,7 @@
         <v>2712</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -27582,7 +27588,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="422" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -27664,7 +27670,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="424" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -27705,7 +27711,7 @@
         <v>2734</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="425" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -27787,7 +27793,7 @@
         <v>2745</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="427" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -27869,7 +27875,7 @@
         <v>2756</v>
       </c>
     </row>
-    <row r="429" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="429" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -27910,7 +27916,7 @@
         <v>2762</v>
       </c>
     </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="430" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -27992,7 +27998,7 @@
         <v>2776</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="432" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -28033,7 +28039,7 @@
         <v>2782</v>
       </c>
     </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="433" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -28074,7 +28080,7 @@
         <v>2788</v>
       </c>
     </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="434" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -28115,7 +28121,7 @@
         <v>2794</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="435" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -28156,7 +28162,7 @@
         <v>2798</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="436" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -28197,7 +28203,7 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="437" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -28238,7 +28244,7 @@
         <v>2809</v>
       </c>
     </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="438" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -28320,7 +28326,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -28361,7 +28367,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="441" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -28402,7 +28408,7 @@
         <v>2832</v>
       </c>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="442" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -28443,7 +28449,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="443" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -28484,7 +28490,7 @@
         <v>2842</v>
       </c>
     </row>
-    <row r="444" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="444" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -28566,7 +28572,7 @@
         <v>2854</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="446" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -28607,7 +28613,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="447" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="447" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A447" s="1">
         <v>445</v>
       </c>
@@ -28648,7 +28654,7 @@
         <v>2868</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A448" s="1">
         <v>446</v>
       </c>
@@ -28689,7 +28695,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="449" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A449" s="1">
         <v>447</v>
       </c>
@@ -28812,7 +28818,7 @@
         <v>2891</v>
       </c>
     </row>
-    <row r="452" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="452" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A452" s="1">
         <v>450</v>
       </c>
@@ -28853,7 +28859,7 @@
         <v>2898</v>
       </c>
     </row>
-    <row r="453" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="453" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -28976,7 +28982,7 @@
         <v>2916</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="456" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A456" s="1">
         <v>454</v>
       </c>
@@ -29017,7 +29023,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="457" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A457" s="1">
         <v>455</v>
       </c>
@@ -29058,7 +29064,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="458" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="458" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A458" s="1">
         <v>456</v>
       </c>
@@ -29099,7 +29105,7 @@
         <v>2935</v>
       </c>
     </row>
-    <row r="459" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="459" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A459" s="1">
         <v>457</v>
       </c>
@@ -29140,7 +29146,7 @@
         <v>2939</v>
       </c>
     </row>
-    <row r="460" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="460" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -29181,7 +29187,7 @@
         <v>2946</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="461" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A461" s="1">
         <v>459</v>
       </c>
@@ -29222,7 +29228,7 @@
         <v>2951</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="462" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A462" s="1">
         <v>460</v>
       </c>
@@ -29263,7 +29269,7 @@
         <v>2957</v>
       </c>
     </row>
-    <row r="463" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="463" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A463" s="1">
         <v>461</v>
       </c>
@@ -29304,7 +29310,7 @@
         <v>2963</v>
       </c>
     </row>
-    <row r="464" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="464" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A464" s="1">
         <v>462</v>
       </c>
@@ -29345,7 +29351,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="465" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="465" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A465" s="1">
         <v>463</v>
       </c>
@@ -29386,7 +29392,7 @@
         <v>2974</v>
       </c>
     </row>
-    <row r="466" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="466" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A466" s="1">
         <v>464</v>
       </c>
@@ -29427,7 +29433,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="467" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="467" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A467" s="1">
         <v>465</v>
       </c>
@@ -29468,7 +29474,7 @@
         <v>2986</v>
       </c>
     </row>
-    <row r="468" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="468" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -29509,7 +29515,7 @@
         <v>2992</v>
       </c>
     </row>
-    <row r="469" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="469" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A469" s="1">
         <v>467</v>
       </c>
@@ -29550,7 +29556,7 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="470" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="470" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A470" s="1">
         <v>468</v>
       </c>
@@ -29632,7 +29638,7 @@
         <v>3009</v>
       </c>
     </row>
-    <row r="472" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="472" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A472" s="1">
         <v>470</v>
       </c>
@@ -29673,7 +29679,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="473" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="473" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A473" s="1">
         <v>471</v>
       </c>
@@ -29796,7 +29802,7 @@
         <v>3033</v>
       </c>
     </row>
-    <row r="476" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="476" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A476" s="1">
         <v>474</v>
       </c>
@@ -29837,7 +29843,7 @@
         <v>3039</v>
       </c>
     </row>
-    <row r="477" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="477" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A477" s="1">
         <v>475</v>
       </c>
@@ -29919,7 +29925,7 @@
         <v>3051</v>
       </c>
     </row>
-    <row r="479" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="479" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A479" s="1">
         <v>477</v>
       </c>
@@ -29960,7 +29966,7 @@
         <v>3057</v>
       </c>
     </row>
-    <row r="480" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="480" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A480" s="1">
         <v>478</v>
       </c>
@@ -30001,7 +30007,7 @@
         <v>3063</v>
       </c>
     </row>
-    <row r="481" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="481" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A481" s="1">
         <v>479</v>
       </c>
@@ -30083,7 +30089,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="483" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="483" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A483" s="1">
         <v>481</v>
       </c>
@@ -30165,7 +30171,7 @@
         <v>3087</v>
       </c>
     </row>
-    <row r="485" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="485" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A485" s="1">
         <v>483</v>
       </c>
@@ -30206,7 +30212,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="486" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="486" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A486" s="1">
         <v>484</v>
       </c>
@@ -30247,7 +30253,7 @@
         <v>3099</v>
       </c>
     </row>
-    <row r="487" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="487" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A487" s="1">
         <v>485</v>
       </c>
@@ -30288,7 +30294,7 @@
         <v>3104</v>
       </c>
     </row>
-    <row r="488" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="488" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A488" s="1">
         <v>486</v>
       </c>
@@ -30329,7 +30335,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="489" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="489" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A489" s="1">
         <v>487</v>
       </c>
@@ -30370,7 +30376,7 @@
         <v>3117</v>
       </c>
     </row>
-    <row r="490" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="490" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A490" s="1">
         <v>488</v>
       </c>
@@ -30411,7 +30417,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="491" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="491" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A491" s="1">
         <v>489</v>
       </c>
@@ -30452,7 +30458,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="492" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="492" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A492" s="1">
         <v>490</v>
       </c>
@@ -30493,7 +30499,7 @@
         <v>3133</v>
       </c>
     </row>
-    <row r="493" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="493" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A493" s="1">
         <v>491</v>
       </c>
@@ -30534,7 +30540,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="494" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="494" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A494" s="1">
         <v>492</v>
       </c>
@@ -30575,7 +30581,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="495" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="495" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A495" s="1">
         <v>493</v>
       </c>
@@ -30616,7 +30622,7 @@
         <v>3149</v>
       </c>
     </row>
-    <row r="496" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="496" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A496" s="1">
         <v>494</v>
       </c>
@@ -30657,7 +30663,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="497" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="497" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A497" s="1">
         <v>495</v>
       </c>
@@ -30698,7 +30704,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="498" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="498" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A498" s="1">
         <v>496</v>
       </c>
@@ -30739,7 +30745,7 @@
         <v>3166</v>
       </c>
     </row>
-    <row r="499" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="499" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A499" s="1">
         <v>497</v>
       </c>
@@ -30780,7 +30786,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="500" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="500" spans="1:13" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A500" s="1">
         <v>498</v>
       </c>
@@ -30863,6 +30869,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M501" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>